<commit_message>
ETL enabled and corrections on TS levels
ETL is enabled for heat pumps
Electric and hydrogen technologies are on daynite TS level now.
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SuppXLS/Scen_X_ELCCO2_Constraints.xlsx
+++ b/TIMES-NZ/SuppXLS/Scen_X_ELCCO2_Constraints.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suleimenov_b\switchdrive\TIMES_NZ_II\Model_versions\NZ_TIMES-v52\NZ_TIMES_model-v52\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\TIMES-NZ-Model-Files\TIMES-NZ\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045FDE55-EF7D-4DD4-838A-ED9F98EA76B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="11565"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2 Limit" sheetId="1" r:id="rId1"/>
     <sheet name="Emissions" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="78">
   <si>
     <t>LimType</t>
   </si>
@@ -53,12 +67,6 @@
     <t>UC_COMNET</t>
   </si>
   <si>
-    <t>UC_RHSTS</t>
-  </si>
-  <si>
-    <t>UC_RHSTS~0</t>
-  </si>
-  <si>
     <t>UC_Desc</t>
   </si>
   <si>
@@ -66,9 +74,6 @@
   </si>
   <si>
     <t>~UC_Sets: R_S: AllRegions</t>
-  </si>
-  <si>
-    <t>~UC_Sets: T_S:</t>
   </si>
   <si>
     <t>Energy sector greenhouse gas emissions</t>
@@ -283,17 +288,26 @@
   <si>
     <t>UC_T</t>
   </si>
+  <si>
+    <t>UC_RHST</t>
+  </si>
+  <si>
+    <t>UC_RHST~0</t>
+  </si>
+  <si>
+    <t>~UC_Sets: T_E:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00;\-#,##0.00;\-"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1567,10 +1581,10 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="29" borderId="12" xfId="229" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="29" borderId="12" xfId="229" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="33" fillId="29" borderId="12" xfId="229" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1579,11 +1593,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="29" borderId="13" xfId="229" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="32" fillId="29" borderId="15" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="229" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="29" borderId="16" xfId="229" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1607,7 +1621,7 @@
     <xf numFmtId="166" fontId="32" fillId="29" borderId="17" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="32" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="32" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="32" fillId="29" borderId="12" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1622,7 +1636,7 @@
     <xf numFmtId="166" fontId="34" fillId="29" borderId="17" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="34" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="34" fillId="29" borderId="12" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1637,7 +1651,7 @@
     <xf numFmtId="166" fontId="33" fillId="29" borderId="17" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="33" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="33" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="33" fillId="29" borderId="12" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1652,7 +1666,7 @@
     <xf numFmtId="166" fontId="36" fillId="29" borderId="17" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="36" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="36" fillId="29" borderId="0" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="36" fillId="29" borderId="12" xfId="229" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1706,237 +1720,237 @@
     </xf>
   </cellXfs>
   <cellStyles count="231">
-    <cellStyle name="20% - Accent1 2" xfId="4"/>
-    <cellStyle name="20% - Accent2 2" xfId="5"/>
-    <cellStyle name="20% - Accent3 2" xfId="6"/>
-    <cellStyle name="20% - Accent4 2" xfId="7"/>
-    <cellStyle name="20% - Accent5 2" xfId="8"/>
-    <cellStyle name="20% - Accent6 2" xfId="9"/>
-    <cellStyle name="20% - Akzent1" xfId="10"/>
-    <cellStyle name="20% - Akzent2" xfId="11"/>
-    <cellStyle name="20% - Akzent3" xfId="12"/>
-    <cellStyle name="20% - Akzent4" xfId="13"/>
-    <cellStyle name="20% - Akzent5" xfId="14"/>
-    <cellStyle name="20% - Akzent6" xfId="15"/>
-    <cellStyle name="40% - Accent1 2" xfId="16"/>
-    <cellStyle name="40% - Accent2 2" xfId="17"/>
-    <cellStyle name="40% - Accent3 2" xfId="18"/>
-    <cellStyle name="40% - Accent4 2" xfId="19"/>
-    <cellStyle name="40% - Accent5 2" xfId="20"/>
-    <cellStyle name="40% - Accent6 2" xfId="21"/>
-    <cellStyle name="40% - Akzent1" xfId="22"/>
-    <cellStyle name="40% - Akzent2" xfId="23"/>
-    <cellStyle name="40% - Akzent3" xfId="24"/>
-    <cellStyle name="40% - Akzent4" xfId="25"/>
-    <cellStyle name="40% - Akzent5" xfId="26"/>
-    <cellStyle name="40% - Akzent6" xfId="27"/>
-    <cellStyle name="60% - Accent1 2" xfId="28"/>
-    <cellStyle name="60% - Accent2 2" xfId="29"/>
-    <cellStyle name="60% - Accent3 2" xfId="30"/>
-    <cellStyle name="60% - Accent4 2" xfId="31"/>
-    <cellStyle name="60% - Accent5 2" xfId="32"/>
-    <cellStyle name="60% - Accent6 2" xfId="33"/>
-    <cellStyle name="60% - Akzent1" xfId="34"/>
-    <cellStyle name="60% - Akzent2" xfId="35"/>
-    <cellStyle name="60% - Akzent3" xfId="36"/>
-    <cellStyle name="60% - Akzent4" xfId="37"/>
-    <cellStyle name="60% - Akzent5" xfId="38"/>
-    <cellStyle name="60% - Akzent6" xfId="39"/>
-    <cellStyle name="Accent1 2" xfId="40"/>
-    <cellStyle name="Accent2 2" xfId="41"/>
-    <cellStyle name="Accent3 2" xfId="42"/>
-    <cellStyle name="Accent4 2" xfId="43"/>
-    <cellStyle name="Accent5 2" xfId="44"/>
-    <cellStyle name="Accent6 2" xfId="45"/>
-    <cellStyle name="Akzent1" xfId="46"/>
-    <cellStyle name="Akzent2" xfId="47"/>
-    <cellStyle name="Akzent3" xfId="48"/>
-    <cellStyle name="Akzent4" xfId="49"/>
-    <cellStyle name="Akzent5" xfId="50"/>
-    <cellStyle name="Akzent6" xfId="51"/>
-    <cellStyle name="Ausgabe" xfId="52"/>
-    <cellStyle name="Bad 2" xfId="53"/>
-    <cellStyle name="Berechnung" xfId="54"/>
-    <cellStyle name="Calculation 2" xfId="55"/>
-    <cellStyle name="Check Cell 2" xfId="56"/>
-    <cellStyle name="Comma 2" xfId="57"/>
-    <cellStyle name="Comma 3" xfId="58"/>
-    <cellStyle name="Eingabe" xfId="59"/>
-    <cellStyle name="Ergebnis" xfId="60"/>
-    <cellStyle name="Erklärender Text" xfId="61"/>
-    <cellStyle name="Euro" xfId="62"/>
-    <cellStyle name="Euro 2" xfId="63"/>
-    <cellStyle name="Explanatory Text 2" xfId="64"/>
-    <cellStyle name="Float" xfId="65"/>
-    <cellStyle name="Float 2" xfId="66"/>
-    <cellStyle name="Good 2" xfId="67"/>
-    <cellStyle name="Gut" xfId="68"/>
-    <cellStyle name="Heading 1 2" xfId="69"/>
-    <cellStyle name="Heading 2 2" xfId="70"/>
-    <cellStyle name="Heading 3 2" xfId="71"/>
-    <cellStyle name="Heading 4 2" xfId="72"/>
-    <cellStyle name="Input 2" xfId="73"/>
-    <cellStyle name="Komma 5" xfId="74"/>
-    <cellStyle name="Linked Cell 2" xfId="75"/>
-    <cellStyle name="Neutral 2" xfId="76"/>
+    <cellStyle name="20% - Accent1 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - Akzent1" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Akzent2" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Akzent3" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - Akzent4" xfId="13" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - Akzent5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Akzent6" xfId="15" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="40% - Akzent1" xfId="22" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="40% - Akzent2" xfId="23" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - Akzent3" xfId="24" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="40% - Akzent4" xfId="25" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="40% - Akzent5" xfId="26" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="40% - Akzent6" xfId="27" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="60% - Akzent1" xfId="34" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="60% - Akzent2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="60% - Akzent3" xfId="36" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="60% - Akzent4" xfId="37" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="60% - Akzent5" xfId="38" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="60% - Akzent6" xfId="39" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Accent1 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Accent2 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Accent3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Accent4 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Accent5 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Accent6 2" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Akzent1" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Akzent2" xfId="47" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Akzent3" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Akzent4" xfId="49" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Akzent5" xfId="50" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Akzent6" xfId="51" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Ausgabe" xfId="52" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Bad 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Berechnung" xfId="54" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Calculation 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Check Cell 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Comma 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Comma 3" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Eingabe" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Ergebnis" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Erklärender Text" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Euro" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Euro 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Float" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Float 2" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Good 2" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Gut" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Heading 1 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Heading 2 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Heading 3 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Heading 4 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Komma 5" xfId="74" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Neutral 2" xfId="76" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="229"/>
-    <cellStyle name="Normal 2" xfId="77"/>
-    <cellStyle name="Normal 3" xfId="78"/>
-    <cellStyle name="Normal 4" xfId="79"/>
-    <cellStyle name="Normal 4 2" xfId="80"/>
-    <cellStyle name="Normal 4_AFs" xfId="81"/>
-    <cellStyle name="Normal 5" xfId="82"/>
-    <cellStyle name="Normal 6" xfId="83"/>
-    <cellStyle name="Normal 7" xfId="84"/>
-    <cellStyle name="Normal 8" xfId="85"/>
-    <cellStyle name="Normal 9" xfId="86"/>
-    <cellStyle name="Normale_B2020" xfId="87"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="2"/>
-    <cellStyle name="Note 2" xfId="88"/>
-    <cellStyle name="Notiz" xfId="89"/>
-    <cellStyle name="Notiz 2" xfId="90"/>
-    <cellStyle name="Output 2" xfId="91"/>
-    <cellStyle name="Percent 2" xfId="92"/>
-    <cellStyle name="Percent 3" xfId="230"/>
-    <cellStyle name="Schlecht" xfId="93"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="94"/>
-    <cellStyle name="Style 103" xfId="95"/>
-    <cellStyle name="Style 103 2" xfId="96"/>
-    <cellStyle name="Style 104" xfId="97"/>
-    <cellStyle name="Style 104 2" xfId="98"/>
-    <cellStyle name="Style 105" xfId="99"/>
-    <cellStyle name="Style 106" xfId="100"/>
-    <cellStyle name="Style 107" xfId="101"/>
-    <cellStyle name="Style 108" xfId="102"/>
-    <cellStyle name="Style 108 2" xfId="103"/>
-    <cellStyle name="Style 109" xfId="104"/>
-    <cellStyle name="Style 110" xfId="105"/>
-    <cellStyle name="Style 114" xfId="106"/>
-    <cellStyle name="Style 114 2" xfId="107"/>
-    <cellStyle name="Style 115" xfId="108"/>
-    <cellStyle name="Style 115 2" xfId="109"/>
-    <cellStyle name="Style 116" xfId="110"/>
-    <cellStyle name="Style 117" xfId="111"/>
-    <cellStyle name="Style 118" xfId="112"/>
-    <cellStyle name="Style 119" xfId="113"/>
-    <cellStyle name="Style 119 2" xfId="114"/>
-    <cellStyle name="Style 120" xfId="115"/>
-    <cellStyle name="Style 121" xfId="116"/>
-    <cellStyle name="Style 126" xfId="117"/>
-    <cellStyle name="Style 126 2" xfId="118"/>
-    <cellStyle name="Style 127" xfId="119"/>
-    <cellStyle name="Style 128" xfId="120"/>
-    <cellStyle name="Style 129" xfId="121"/>
-    <cellStyle name="Style 130" xfId="122"/>
-    <cellStyle name="Style 130 2" xfId="123"/>
-    <cellStyle name="Style 131" xfId="124"/>
-    <cellStyle name="Style 132" xfId="125"/>
-    <cellStyle name="Style 137" xfId="126"/>
-    <cellStyle name="Style 137 2" xfId="127"/>
-    <cellStyle name="Style 138" xfId="128"/>
-    <cellStyle name="Style 139" xfId="129"/>
-    <cellStyle name="Style 140" xfId="130"/>
-    <cellStyle name="Style 141" xfId="131"/>
-    <cellStyle name="Style 141 2" xfId="132"/>
-    <cellStyle name="Style 142" xfId="133"/>
-    <cellStyle name="Style 143" xfId="134"/>
-    <cellStyle name="Style 148" xfId="135"/>
-    <cellStyle name="Style 148 2" xfId="136"/>
-    <cellStyle name="Style 149" xfId="137"/>
-    <cellStyle name="Style 150" xfId="138"/>
-    <cellStyle name="Style 151" xfId="139"/>
-    <cellStyle name="Style 152" xfId="140"/>
-    <cellStyle name="Style 152 2" xfId="141"/>
-    <cellStyle name="Style 153" xfId="142"/>
-    <cellStyle name="Style 154" xfId="143"/>
-    <cellStyle name="Style 159" xfId="144"/>
-    <cellStyle name="Style 159 2" xfId="145"/>
-    <cellStyle name="Style 160" xfId="146"/>
-    <cellStyle name="Style 161" xfId="147"/>
-    <cellStyle name="Style 162" xfId="148"/>
-    <cellStyle name="Style 163" xfId="149"/>
-    <cellStyle name="Style 163 2" xfId="150"/>
-    <cellStyle name="Style 164" xfId="151"/>
-    <cellStyle name="Style 165" xfId="152"/>
-    <cellStyle name="Style 21" xfId="153"/>
-    <cellStyle name="Style 21 2" xfId="154"/>
-    <cellStyle name="Style 22" xfId="155"/>
-    <cellStyle name="Style 23" xfId="156"/>
-    <cellStyle name="Style 24" xfId="157"/>
-    <cellStyle name="Style 25" xfId="158"/>
-    <cellStyle name="Style 25 2" xfId="159"/>
-    <cellStyle name="Style 26" xfId="160"/>
-    <cellStyle name="Style 27" xfId="161"/>
-    <cellStyle name="Style 35" xfId="162"/>
-    <cellStyle name="Style 35 2" xfId="163"/>
-    <cellStyle name="Style 36" xfId="164"/>
-    <cellStyle name="Style 37" xfId="165"/>
-    <cellStyle name="Style 38" xfId="166"/>
-    <cellStyle name="Style 39" xfId="167"/>
-    <cellStyle name="Style 39 2" xfId="168"/>
-    <cellStyle name="Style 40" xfId="169"/>
-    <cellStyle name="Style 41" xfId="170"/>
-    <cellStyle name="Style 46" xfId="171"/>
-    <cellStyle name="Style 46 2" xfId="172"/>
-    <cellStyle name="Style 47" xfId="173"/>
-    <cellStyle name="Style 48" xfId="174"/>
-    <cellStyle name="Style 49" xfId="175"/>
-    <cellStyle name="Style 50" xfId="176"/>
-    <cellStyle name="Style 50 2" xfId="177"/>
-    <cellStyle name="Style 51" xfId="178"/>
-    <cellStyle name="Style 52" xfId="179"/>
-    <cellStyle name="Style 58" xfId="180"/>
-    <cellStyle name="Style 58 2" xfId="181"/>
-    <cellStyle name="Style 59" xfId="182"/>
-    <cellStyle name="Style 60" xfId="183"/>
-    <cellStyle name="Style 61" xfId="184"/>
-    <cellStyle name="Style 62" xfId="185"/>
-    <cellStyle name="Style 62 2" xfId="186"/>
-    <cellStyle name="Style 63" xfId="187"/>
-    <cellStyle name="Style 64" xfId="188"/>
-    <cellStyle name="Style 69" xfId="189"/>
-    <cellStyle name="Style 69 2" xfId="190"/>
-    <cellStyle name="Style 70" xfId="191"/>
-    <cellStyle name="Style 71" xfId="192"/>
-    <cellStyle name="Style 72" xfId="193"/>
-    <cellStyle name="Style 73" xfId="194"/>
-    <cellStyle name="Style 73 2" xfId="195"/>
-    <cellStyle name="Style 74" xfId="196"/>
-    <cellStyle name="Style 75" xfId="197"/>
-    <cellStyle name="Style 80" xfId="198"/>
-    <cellStyle name="Style 80 2" xfId="199"/>
-    <cellStyle name="Style 81" xfId="200"/>
-    <cellStyle name="Style 81 2" xfId="201"/>
-    <cellStyle name="Style 82" xfId="202"/>
-    <cellStyle name="Style 83" xfId="203"/>
-    <cellStyle name="Style 84" xfId="204"/>
-    <cellStyle name="Style 85" xfId="205"/>
-    <cellStyle name="Style 85 2" xfId="206"/>
-    <cellStyle name="Style 86" xfId="207"/>
-    <cellStyle name="Style 87" xfId="208"/>
-    <cellStyle name="Style 93" xfId="209"/>
-    <cellStyle name="Style 93 2" xfId="210"/>
-    <cellStyle name="Style 94" xfId="211"/>
-    <cellStyle name="Style 95" xfId="212"/>
-    <cellStyle name="Style 96" xfId="213"/>
-    <cellStyle name="Style 97" xfId="214"/>
-    <cellStyle name="Style 97 2" xfId="215"/>
-    <cellStyle name="Style 98" xfId="216"/>
-    <cellStyle name="Style 99" xfId="217"/>
-    <cellStyle name="Title 2" xfId="218"/>
-    <cellStyle name="Total 2" xfId="219"/>
-    <cellStyle name="Überschrift" xfId="220"/>
-    <cellStyle name="Überschrift 1" xfId="221"/>
-    <cellStyle name="Überschrift 2" xfId="222"/>
-    <cellStyle name="Überschrift 3" xfId="223"/>
-    <cellStyle name="Überschrift 4" xfId="224"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="225"/>
-    <cellStyle name="Warnender Text" xfId="226"/>
-    <cellStyle name="Warning Text 2" xfId="227"/>
-    <cellStyle name="Zelle überprüfen" xfId="228"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 12" xfId="229" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 3" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 4" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 4 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 4_AFs" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 5" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 6" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 7" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 8" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 9" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normale_B2020" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="2" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Note 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Notiz" xfId="89" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Notiz 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Output 2" xfId="91" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Percent 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Percent 3" xfId="230" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Schlecht" xfId="93" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="94" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Style 103" xfId="95" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Style 103 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Style 104" xfId="97" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Style 104 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Style 105" xfId="99" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Style 106" xfId="100" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Style 107" xfId="101" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Style 108" xfId="102" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Style 108 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Style 109" xfId="104" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Style 110" xfId="105" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Style 114" xfId="106" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Style 114 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Style 115" xfId="108" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Style 115 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Style 116" xfId="110" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Style 117" xfId="111" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Style 118" xfId="112" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Style 119" xfId="113" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Style 119 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Style 120" xfId="115" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Style 121" xfId="116" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Style 126" xfId="117" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Style 126 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Style 127" xfId="119" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Style 128" xfId="120" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Style 129" xfId="121" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Style 130" xfId="122" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Style 130 2" xfId="123" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Style 131" xfId="124" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Style 132" xfId="125" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Style 137" xfId="126" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Style 137 2" xfId="127" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Style 138" xfId="128" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Style 139" xfId="129" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Style 140" xfId="130" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Style 141" xfId="131" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="Style 141 2" xfId="132" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Style 142" xfId="133" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Style 143" xfId="134" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Style 148" xfId="135" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Style 148 2" xfId="136" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Style 149" xfId="137" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Style 150" xfId="138" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Style 151" xfId="139" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Style 152" xfId="140" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Style 152 2" xfId="141" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Style 153" xfId="142" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Style 154" xfId="143" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Style 159" xfId="144" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Style 159 2" xfId="145" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Style 160" xfId="146" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Style 161" xfId="147" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Style 162" xfId="148" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Style 163" xfId="149" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Style 163 2" xfId="150" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Style 164" xfId="151" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="Style 165" xfId="152" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Style 21" xfId="153" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="Style 21 2" xfId="154" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="Style 22" xfId="155" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="Style 23" xfId="156" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="Style 24" xfId="157" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="Style 25" xfId="158" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="Style 25 2" xfId="159" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="Style 26" xfId="160" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="Style 27" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="Style 35" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="Style 35 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="Style 36" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="Style 37" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="Style 38" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="Style 39" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="Style 39 2" xfId="168" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="Style 40" xfId="169" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="Style 41" xfId="170" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="Style 46" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="Style 46 2" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="Style 47" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="Style 48" xfId="174" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="Style 49" xfId="175" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="Style 50" xfId="176" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="Style 50 2" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="Style 51" xfId="178" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="Style 52" xfId="179" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="Style 58" xfId="180" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="Style 58 2" xfId="181" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="Style 59" xfId="182" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="Style 60" xfId="183" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="Style 61" xfId="184" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="Style 62" xfId="185" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="Style 62 2" xfId="186" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="Style 63" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="Style 64" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="Style 69" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="Style 69 2" xfId="190" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="Style 70" xfId="191" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="Style 71" xfId="192" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="Style 72" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="Style 73" xfId="194" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="Style 73 2" xfId="195" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="Style 74" xfId="196" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="Style 75" xfId="197" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="Style 80" xfId="198" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="Style 80 2" xfId="199" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="Style 81" xfId="200" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="Style 81 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="Style 82" xfId="202" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="Style 83" xfId="203" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="Style 84" xfId="204" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="Style 85" xfId="205" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="Style 85 2" xfId="206" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="Style 86" xfId="207" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="Style 87" xfId="208" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="Style 93" xfId="209" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="Style 93 2" xfId="210" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="Style 94" xfId="211" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="Style 95" xfId="212" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="Style 96" xfId="213" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="Style 97" xfId="214" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="Style 97 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="Style 98" xfId="216" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="Style 99" xfId="217" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="Title 2" xfId="218" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="Total 2" xfId="219" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="Überschrift" xfId="220" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="Überschrift 1" xfId="221" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="Überschrift 2" xfId="222" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="Überschrift 3" xfId="223" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="Überschrift 4" xfId="224" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="225" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="Warnender Text" xfId="226" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="Warning Text 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="Zelle überprüfen" xfId="228" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1952,9 +1966,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1992,9 +2006,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2029,7 +2043,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2064,7 +2078,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2237,31 +2251,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="13" width="15.7109375" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.1796875" style="2"/>
+    <col min="3" max="13" width="15.7265625" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="8" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="C4" s="1"/>
       <c r="I4" s="2" t="s">
         <v>3</v>
@@ -2271,7 +2285,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2297,23 +2311,23 @@
         <v>9</v>
       </c>
       <c r="K5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:13">
+      <c r="C6" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="7">
@@ -2334,83 +2348,75 @@
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="7">
         <v>2030</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="6">
-        <v>1</v>
-      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="75">
-        <f>+Emissions!Q8*0.7</f>
-        <v>22951.319114376627</v>
+        <f>+Emissions!Q8*0.6</f>
+        <v>19672.55924089425</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="7">
         <v>2050</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="75">
-        <f>+Emissions!B8*0.5</f>
-        <v>11221.291572560918</v>
+        <f>+Emissions!B8*0.2</f>
+        <v>4488.5166290243678</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13">
       <c r="C18" s="1"/>
       <c r="I18" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13">
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
@@ -2436,23 +2442,23 @@
         <v>9</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13">
       <c r="C20" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="7"/>
@@ -2471,7 +2477,7 @@
       </c>
       <c r="M20" s="6"/>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -2484,7 +2490,7 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2504,27 +2510,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:AF102"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10.5"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="12" customWidth="1"/>
-    <col min="2" max="28" width="10.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="9.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="40.453125" style="12" customWidth="1"/>
+    <col min="2" max="28" width="10.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="9.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.1796875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32">
       <c r="A1" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2558,9 +2564,9 @@
       <c r="AE1" s="11"/>
       <c r="AF1" s="11"/>
     </row>
-    <row r="2" spans="1:32" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="12.5">
       <c r="A2" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -2594,7 +2600,7 @@
       <c r="AE2" s="11"/>
       <c r="AF2" s="11"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32">
       <c r="A3" s="14"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -2628,7 +2634,7 @@
       <c r="AE3" s="11"/>
       <c r="AF3" s="11"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -2662,7 +2668,7 @@
       <c r="AE4" s="17"/>
       <c r="AF4" s="17"/>
     </row>
-    <row r="5" spans="1:32" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="31.5">
       <c r="A5" s="14"/>
       <c r="B5" s="18">
         <v>1990</v>
@@ -2746,19 +2752,19 @@
         <v>2016</v>
       </c>
       <c r="AC5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AD5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="AE5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF5" s="21" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="11" thickBot="1">
       <c r="A6" s="14"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2792,9 +2798,9 @@
       <c r="AE6" s="11"/>
       <c r="AF6" s="23"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32">
       <c r="A7" s="24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="25">
         <v>23779.701368662241</v>
@@ -2888,9 +2894,9 @@
       </c>
       <c r="AF7" s="30"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="31">
         <v>22442.583145121836</v>
@@ -2986,9 +2992,9 @@
         <v>0.93578301365627692</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32">
       <c r="A9" s="37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="38">
         <v>6003.8998042934982</v>
@@ -3084,9 +3090,9 @@
         <v>0.13307609101123216</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32">
       <c r="A10" s="44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="45">
         <v>3502.2600399409166</v>
@@ -3182,9 +3188,9 @@
         <v>9.7144843147341148E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32">
       <c r="A11" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="52">
         <v>3014.5493313361899</v>
@@ -3280,9 +3286,9 @@
         <v>8.2777825678383127E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32">
       <c r="A12" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="52">
         <v>477.09141807639998</v>
@@ -3378,9 +3384,9 @@
         <v>1.4318625885696514E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32">
       <c r="A13" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B13" s="52">
         <v>10.603560160927101</v>
@@ -3476,9 +3482,9 @@
         <v>4.495932521708626E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32">
       <c r="A14" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B14" s="52">
         <v>1.57303674E-2</v>
@@ -3574,9 +3580,9 @@
         <v>3.4322580444118397E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32">
       <c r="A15" s="44" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="45">
         <v>780.04528007816396</v>
@@ -3672,9 +3678,9 @@
         <v>2.712214412304392E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32">
       <c r="A16" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="52">
         <v>0</v>
@@ -3758,10 +3764,10 @@
         <v>157.20751626720099</v>
       </c>
       <c r="AC16" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD16" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE16" s="56">
         <v>0.45598345271020935</v>
@@ -3770,9 +3776,9 @@
         <v>5.0259174617273894E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32">
       <c r="A17" s="51" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="52">
         <v>780.04528007816396</v>
@@ -3868,9 +3874,9 @@
         <v>2.2096226661316533E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32">
       <c r="A18" s="44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="45">
         <v>1496.25935688865</v>
@@ -3960,15 +3966,15 @@
         <v>-1</v>
       </c>
       <c r="AE18" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF18" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32">
+      <c r="A19" s="44" t="s">
         <v>30</v>
-      </c>
-      <c r="AF18" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
-        <v>33</v>
       </c>
       <c r="B19" s="45">
         <v>225.335127385768</v>
@@ -4064,9 +4070,9 @@
         <v>8.8091037408470924E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32">
       <c r="A20" s="51" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" s="52">
         <v>0</v>
@@ -4150,10 +4156,10 @@
         <v>1.98538085733333</v>
       </c>
       <c r="AC20" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD20" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE20" s="56">
         <v>1.1845887963289949</v>
@@ -4162,9 +4168,9 @@
         <v>6.3472539710448403E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32">
       <c r="A21" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="52">
         <v>225.335127385768</v>
@@ -4260,9 +4266,9 @@
         <v>8.745631201136644E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32">
       <c r="A22" s="37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B22" s="38">
         <v>4760.2487736156218</v>
@@ -4358,9 +4364,9 @@
         <v>0.22079213039838189</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32">
       <c r="A23" s="44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="45">
         <v>367.64256400825298</v>
@@ -4456,9 +4462,9 @@
         <v>1.7645379679417886E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32">
       <c r="A24" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24" s="52">
         <v>10.7507686864639</v>
@@ -4554,9 +4560,9 @@
         <v>1.0668196911029577E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32">
       <c r="A25" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25" s="52">
         <v>20.051870839962099</v>
@@ -4646,15 +4652,15 @@
         <v>-1</v>
       </c>
       <c r="AE25" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AF25" s="57">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32">
       <c r="A26" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" s="52">
         <v>336.83992448182698</v>
@@ -4750,9 +4756,9 @@
         <v>1.657855998831493E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32">
       <c r="A27" s="44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B27" s="45">
         <v>553.21671671388049</v>
@@ -4848,9 +4854,9 @@
         <v>6.2959183646947692E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32">
       <c r="A28" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" s="52">
         <v>529.18972884855395</v>
@@ -4946,9 +4952,9 @@
         <v>6.2060879874952041E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32">
       <c r="A29" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="52">
         <v>0</v>
@@ -5032,10 +5038,10 @@
         <v>0.17027240151370199</v>
       </c>
       <c r="AC29" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD29" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE29" s="56">
         <v>-0.14242130017646748</v>
@@ -5044,9 +5050,9 @@
         <v>5.443601275166998E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32">
       <c r="A30" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="52">
         <v>24.0269878653265</v>
@@ -5142,9 +5148,9 @@
         <v>8.9286017072048277E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32">
       <c r="A31" s="44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31" s="45">
         <v>558.70129600516987</v>
@@ -5240,9 +5246,9 @@
         <v>1.8505829986094239E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32">
       <c r="A32" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32" s="52">
         <v>348.88858926847303</v>
@@ -5338,9 +5344,9 @@
         <v>1.149478238457897E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32">
       <c r="A33" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B33" s="52">
         <v>110.25032265879</v>
@@ -5436,9 +5442,9 @@
         <v>1.7583011004961859E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32">
       <c r="A34" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B34" s="52">
         <v>52.579029743385099</v>
@@ -5534,9 +5540,9 @@
         <v>2.7629778880361826E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32">
       <c r="A35" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B35" s="52">
         <v>46.9833543345217</v>
@@ -5632,9 +5638,9 @@
         <v>2.4897686129828978E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32">
       <c r="A36" s="44" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="45">
         <v>1658.5937187468255</v>
@@ -5730,9 +5736,9 @@
         <v>8.9047955209080626E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32">
       <c r="A37" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B37" s="52">
         <v>445.93669422245398</v>
@@ -5828,9 +5834,9 @@
         <v>2.7656121523832497E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32">
       <c r="A38" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B38" s="52">
         <v>945.31776947281799</v>
@@ -5926,9 +5932,9 @@
         <v>4.8187386983079547E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32">
       <c r="A39" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B39" s="52">
         <v>267.31787772469397</v>
@@ -6024,9 +6030,9 @@
         <v>1.3203206477099858E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32">
       <c r="A40" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B40" s="52">
         <v>2.13773268594992E-2</v>
@@ -6122,9 +6128,9 @@
         <v>1.240225068726178E-6</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32">
       <c r="A41" s="44" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="45">
         <v>56.374899363496496</v>
@@ -6220,9 +6226,9 @@
         <v>9.0651539528252057E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32">
       <c r="A42" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B42" s="52">
         <v>41.953783610338597</v>
@@ -6318,9 +6324,9 @@
         <v>4.8572047366006872E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32">
       <c r="A43" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B43" s="52">
         <v>1.837243</v>
@@ -6416,9 +6422,9 @@
         <v>4.9372197611979532E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32">
       <c r="A44" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B44" s="52">
         <v>12.5838727531579</v>
@@ -6514,9 +6520,9 @@
         <v>4.1585770186125396E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32">
       <c r="A45" s="44" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B45" s="45">
         <v>102.03996787526799</v>
@@ -6612,9 +6618,9 @@
         <v>1.3022131304181062E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32">
       <c r="A46" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B46" s="52">
         <v>59.216071066009398</v>
@@ -6710,9 +6716,9 @@
         <v>9.6171462461274251E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32">
       <c r="A47" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B47" s="52">
         <v>23.1167110467768</v>
@@ -6808,9 +6814,9 @@
         <v>1.693846164226378E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32">
       <c r="A48" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B48" s="52">
         <v>19.707185762481799</v>
@@ -6906,9 +6912,9 @@
         <v>1.7111388938272602E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:32">
       <c r="A49" s="44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B49" s="45">
         <v>162.97356975845929</v>
@@ -7004,9 +7010,9 @@
         <v>5.2510259632160229E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:32">
       <c r="A50" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B50" s="52">
         <v>135.703222871066</v>
@@ -7102,9 +7108,9 @@
         <v>4.0269864854323286E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:32">
       <c r="A51" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B51" s="52">
         <v>0</v>
@@ -7188,10 +7194,10 @@
         <v>1.02757414401873</v>
       </c>
       <c r="AC51" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD51" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE51" s="56">
         <v>-0.84502014949692406</v>
@@ -7200,9 +7206,9 @@
         <v>3.2851500718740167E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:32">
       <c r="A52" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B52" s="52">
         <v>27.270346887393298</v>
@@ -7298,9 +7304,9 @@
         <v>1.1911879770649546E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:32">
       <c r="A53" s="44" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B53" s="45">
         <v>498.31204298712828</v>
@@ -7396,9 +7402,9 @@
         <v>1.556839067018354E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:32">
       <c r="A54" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B54" s="52">
         <v>64.404331374451004</v>
@@ -7494,9 +7500,9 @@
         <v>2.6254812554761192E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:32">
       <c r="A55" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B55" s="52">
         <v>385.77023614017997</v>
@@ -7592,9 +7598,9 @@
         <v>8.8673853022373621E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:32">
       <c r="A56" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B56" s="52">
         <v>48.1374754724973</v>
@@ -7690,9 +7696,9 @@
         <v>4.0755241124700589E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:32">
       <c r="A57" s="44" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B57" s="45">
         <v>802.39399815714091</v>
@@ -7788,9 +7794,9 @@
         <v>9.6056367177413064E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:32">
       <c r="A58" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B58" s="52">
         <v>14.2468568720356</v>
@@ -7886,9 +7892,9 @@
         <v>2.2722549528890316E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:32">
       <c r="A59" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B59" s="52">
         <v>736.38646252998899</v>
@@ -7984,9 +7990,9 @@
         <v>2.9643595299659597E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:32">
       <c r="A60" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B60" s="52">
         <v>51.756101466951201</v>
@@ -8082,9 +8088,9 @@
         <v>6.4138507023688866E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:32">
       <c r="A61" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B61" s="52">
         <v>4.5772881651568896E-3</v>
@@ -8180,9 +8186,9 @@
         <v>2.0099011755691276E-7</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:32">
       <c r="A62" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B62" s="38">
         <v>8766.746479473064</v>
@@ -8278,9 +8284,9 @@
         <v>0.47952313055779755</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:32">
       <c r="A63" s="44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B63" s="45">
         <v>7475.2586432220278</v>
@@ -8376,9 +8382,9 @@
         <v>0.43518978188256258</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:32">
       <c r="A64" s="51" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B64" s="52">
         <v>5790.5646610440599</v>
@@ -8474,9 +8480,9 @@
         <v>0.2372962721803778</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:32">
       <c r="A65" s="58" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B65" s="52">
         <v>4627.9596592408898</v>
@@ -8572,9 +8578,9 @@
         <v>5.4481725578459914E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:32">
       <c r="A66" s="58" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B66" s="52">
         <v>1162.6050018031699</v>
@@ -8670,9 +8676,9 @@
         <v>0.18281454660191787</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:32">
       <c r="A67" s="51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B67" s="52">
         <v>1433.8775797252299</v>
@@ -8768,9 +8774,9 @@
         <v>0.19725854688798758</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:32">
       <c r="A68" s="51" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B68" s="52">
         <v>148.467572143757</v>
@@ -8866,9 +8872,9 @@
         <v>2.8652062299104267E-5</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:32">
       <c r="A69" s="51" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B69" s="52">
         <v>102.34883030898099</v>
@@ -8964,9 +8970,9 @@
         <v>6.0631075189804696E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:32">
       <c r="A70" s="44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B70" s="45">
         <v>87.651002021632607</v>
@@ -9062,9 +9068,9 @@
         <v>4.6750343657080765E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:32">
       <c r="A71" s="51" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B71" s="52">
         <v>87.651002021632607</v>
@@ -9160,9 +9166,9 @@
         <v>4.6750343657080765E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:32">
       <c r="A72" s="44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B72" s="45">
         <v>948.32782009385198</v>
@@ -9258,9 +9264,9 @@
         <v>2.9941497827160515E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:32">
       <c r="A73" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B73" s="52">
         <v>948.32782009385198</v>
@@ -9356,9 +9362,9 @@
         <v>2.9941497827160515E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:32">
       <c r="A74" s="44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B74" s="45">
         <v>255.509014135553</v>
@@ -9454,9 +9460,9 @@
         <v>9.7168164823663462E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:32">
       <c r="A75" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B75" s="52">
         <v>248.16296346035301</v>
@@ -9552,9 +9558,9 @@
         <v>9.7109445630615895E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:32">
       <c r="A76" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B76" s="52">
         <v>7.3460506751999999</v>
@@ -9650,9 +9656,9 @@
         <v>5.8719193047570545E-6</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:32">
       <c r="A77" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B77" s="38">
         <v>2911.688087739647</v>
@@ -9748,9 +9754,9 @@
         <v>0.10239166168886545</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:32">
       <c r="A78" s="44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B78" s="45">
         <v>1241.320402282804</v>
@@ -9846,9 +9852,9 @@
         <v>4.9785398524703123E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:32">
       <c r="A79" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B79" s="52">
         <v>106.291950881427</v>
@@ -9944,9 +9950,9 @@
         <v>2.7728577953305446E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:32">
       <c r="A80" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B80" s="52">
         <v>38.096789961657002</v>
@@ -10042,9 +10048,9 @@
         <v>3.9672567669324227E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:32">
       <c r="A81" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B81" s="52">
         <v>1096.9316614397201</v>
@@ -10140,9 +10146,9 @@
         <v>4.3045283962440159E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:32">
       <c r="A82" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B82" s="52">
         <v>0</v>
@@ -10226,21 +10232,21 @@
         <v>0</v>
       </c>
       <c r="AC82" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD82" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE82" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AF82" s="57">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:32">
       <c r="A83" s="44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B83" s="45">
         <v>886.26672102870293</v>
@@ -10336,9 +10342,9 @@
         <v>3.2080002048243447E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:32">
       <c r="A84" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B84" s="52">
         <v>236.68821185599799</v>
@@ -10434,9 +10440,9 @@
         <v>1.4089628262207584E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:32">
       <c r="A85" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B85" s="52">
         <v>143.25307320994</v>
@@ -10532,9 +10538,9 @@
         <v>3.2172087317316155E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:32">
       <c r="A86" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B86" s="52">
         <v>506.25606500380599</v>
@@ -10630,9 +10636,9 @@
         <v>1.4771132245141332E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:32">
       <c r="A87" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B87" s="52">
         <v>6.9370958958874407E-2</v>
@@ -10728,9 +10734,9 @@
         <v>2.0328091629173136E-6</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:32">
       <c r="A88" s="44" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B88" s="45">
         <v>784.10096442814029</v>
@@ -10826,9 +10832,9 @@
         <v>2.0526261115918886E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:32">
       <c r="A89" s="51" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B89" s="52">
         <v>186.08944447622699</v>
@@ -10924,9 +10930,9 @@
         <v>1.0999692892075688E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:32">
       <c r="A90" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B90" s="52">
         <v>373.89989589417797</v>
@@ -11022,9 +11028,9 @@
         <v>1.0997614633323327E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:32">
       <c r="A91" s="51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B91" s="52">
         <v>168.00944309887799</v>
@@ -11120,9 +11126,9 @@
         <v>6.6222449110423815E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:32">
       <c r="A92" s="51" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B92" s="52">
         <v>56.102180958857303</v>
@@ -11218,9 +11224,9 @@
         <v>1.8045618494684824E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:32" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" ht="11" thickBot="1">
       <c r="A93" s="59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B93" s="60">
         <v>1337.1182235404035</v>
@@ -11316,9 +11322,9 @@
         <v>6.4216986343723026E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:32">
       <c r="A94" s="66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B94" s="45">
         <v>328.23420307499998</v>
@@ -11414,9 +11420,9 @@
         <v>5.4923964399937819E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:32">
       <c r="A95" s="66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B95" s="45">
         <v>721.04857162781002</v>
@@ -11512,9 +11518,9 @@
         <v>3.1961312267149287E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:32">
       <c r="A96" s="67" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B96" s="52">
         <v>281.43107222596598</v>
@@ -11610,9 +11616,9 @@
         <v>6.6243367386132372E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32">
       <c r="A97" s="67" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B97" s="52">
         <v>295.95872949843903</v>
@@ -11708,9 +11714,9 @@
         <v>2.0902223072264782E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32">
       <c r="A98" s="67" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B98" s="52">
         <v>143.65876990340499</v>
@@ -11806,9 +11812,9 @@
         <v>4.4347524562712666E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32">
       <c r="A99" s="67" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B99" s="52">
         <v>0</v>
@@ -11892,21 +11898,21 @@
         <v>0</v>
       </c>
       <c r="AC99" s="55" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AD99" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AE99" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AF99" s="57">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32">
       <c r="A100" s="66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B100" s="45">
         <v>4.46783883759338</v>
@@ -12002,9 +12008,9 @@
         <v>1.6505024875005417E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:32" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:32" ht="11" thickBot="1">
       <c r="A101" s="66" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B101" s="45">
         <v>283.36761000000001</v>
@@ -12100,9 +12106,9 @@
         <v>2.6598227387829906E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32">
       <c r="A102" s="68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B102" s="69">
         <v>2388.7710669656299</v>
@@ -12205,12 +12211,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>